<commit_message>
update : - add data guru - add data artikel - add data foto, banner, link, profile library and another
</commit_message>
<xml_diff>
--- a/public/assets/import/guru.xlsx
+++ b/public/assets/import/guru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\simpatika\MAN 2 PAREPARE\PROJEK SIATI MADDUPA\UJIAN\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Herd\perpustakaan-digital-parepare\public\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF709FD6-1621-486D-B78D-B96756866E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100B1691-D5FD-4820-879A-EA614C0546BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>NIP/NIK</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>NAMA GURU</t>
   </si>
   <si>
-    <t>PASSWORD</t>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>NIK/NPK</t>
+  </si>
+  <si>
+    <t>MATA PELAJARAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -384,252 +387,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="4" max="4" width="32.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
         <v>3</v>
       </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2"/>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2"/>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>36</v>
-      </c>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>

</xml_diff>